<commit_message>
edit regulation of checking
</commit_message>
<xml_diff>
--- a/excels/AttendanceChecking.xlsx
+++ b/excels/AttendanceChecking.xlsx
@@ -25,9 +25,6 @@
     <t>1 = present</t>
   </si>
   <si>
-    <t>0 = absent</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -449,6 +446,9 @@
   </si>
   <si>
     <t>Nguyễn Phan Hoài</t>
+  </si>
+  <si>
+    <t>blank = absent</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMA74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -949,7 +949,7 @@
     <col min="1" max="1" width="10.25" style="10" customWidth="1"/>
     <col min="2" max="2" width="21.875" style="10" customWidth="1"/>
     <col min="3" max="3" width="15.25" style="10" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14.375" style="10" customWidth="1"/>
     <col min="5" max="1011" width="9.125" style="10" customWidth="1"/>
     <col min="1012" max="1015" width="11.5" style="1" customWidth="1"/>
   </cols>
@@ -983,81 +983,81 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="P5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="V5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="V5" s="9" t="s">
+      <c r="W5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1065,10 +1065,10 @@
         <v>1511844</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="X6">
-        <f>COUNTBLANK(E6:W6)</f>
+        <f t="shared" ref="X6:X37" si="0">COUNTBLANK(E6:W6)</f>
         <v>18</v>
       </c>
     </row>
@@ -1087,10 +1087,10 @@
         <v>1512221</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="X7">
-        <f>COUNTBLANK(E7:W7)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1109,10 +1109,10 @@
         <v>1512396</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="X8">
-        <f>COUNTBLANK(E8:W8)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1131,10 +1131,10 @@
         <v>1512534</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
@@ -1144,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="X9">
-        <f>COUNTBLANK(E9:W9)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1153,10 +1153,10 @@
         <v>1512640</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="X10">
-        <f>COUNTBLANK(E10:W10)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1175,10 +1175,10 @@
         <v>1510335</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D11" s="8">
         <v>2</v>
@@ -1188,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="X11">
-        <f>COUNTBLANK(E11:W11)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1197,10 +1197,10 @@
         <v>1511234</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="D12" s="8">
         <v>2</v>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="X12">
-        <f>COUNTBLANK(E12:W12)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1219,10 +1219,10 @@
         <v>1511908</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D13" s="8">
         <v>2</v>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="X13">
-        <f>COUNTBLANK(E13:W13)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1241,10 +1241,10 @@
         <v>1513218</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="D14" s="8">
         <v>2</v>
@@ -1254,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="X14">
-        <f>COUNTBLANK(E14:W14)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1263,10 +1263,10 @@
         <v>1510806</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D15" s="8">
         <v>2</v>
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="X15">
-        <f>COUNTBLANK(E15:W15)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1285,17 +1285,17 @@
         <v>1510126</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="D16" s="8">
         <v>3</v>
       </c>
       <c r="E16" s="6"/>
       <c r="X16">
-        <f>COUNTBLANK(E16:W16)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1304,17 +1304,17 @@
         <v>1510462</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="D17" s="8">
         <v>3</v>
       </c>
       <c r="E17" s="6"/>
       <c r="X17">
-        <f>COUNTBLANK(E17:W17)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1323,17 +1323,17 @@
         <v>1511766</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="8">
         <v>3</v>
       </c>
       <c r="E18" s="6"/>
       <c r="X18">
-        <f>COUNTBLANK(E18:W18)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1342,10 +1342,10 @@
         <v>1512676</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="D19" s="8">
         <v>3</v>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="X19">
-        <f>COUNTBLANK(E19:W19)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1364,10 +1364,10 @@
         <v>1510827</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="8">
         <v>3</v>
@@ -1377,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="X20">
-        <f>COUNTBLANK(E20:W20)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1386,17 +1386,17 @@
         <v>1510463</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="8">
         <v>4</v>
       </c>
       <c r="E21" s="6"/>
       <c r="X21">
-        <f>COUNTBLANK(E21:W21)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1405,17 +1405,17 @@
         <v>1513031</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="D22" s="8">
         <v>4</v>
       </c>
       <c r="E22" s="6"/>
       <c r="X22">
-        <f>COUNTBLANK(E22:W22)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1424,17 +1424,17 @@
         <v>1514125</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="D23" s="8">
         <v>4</v>
       </c>
       <c r="E23" s="6"/>
       <c r="X23">
-        <f>COUNTBLANK(E23:W23)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1443,17 +1443,17 @@
         <v>1510652</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="D24" s="8">
         <v>4</v>
       </c>
       <c r="E24" s="6"/>
       <c r="X24">
-        <f>COUNTBLANK(E24:W24)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1462,17 +1462,17 @@
         <v>1510698</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="D25" s="8">
         <v>4</v>
       </c>
       <c r="E25" s="6"/>
       <c r="X25">
-        <f>COUNTBLANK(E25:W25)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1481,10 +1481,10 @@
         <v>1510122</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="8">
         <v>5</v>
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="X26">
-        <f>COUNTBLANK(E26:W26)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1503,10 +1503,10 @@
         <v>1511021</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="8">
         <v>5</v>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="X27">
-        <f>COUNTBLANK(E27:W27)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1525,17 +1525,17 @@
         <v>1511149</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="D28" s="8">
         <v>5</v>
       </c>
       <c r="E28" s="6"/>
       <c r="X28">
-        <f>COUNTBLANK(E28:W28)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1544,17 +1544,17 @@
         <v>1512263</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="D29" s="8">
         <v>5</v>
       </c>
       <c r="E29" s="6"/>
       <c r="X29">
-        <f>COUNTBLANK(E29:W29)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1563,10 +1563,10 @@
         <v>1513524</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="D30" s="8">
         <v>5</v>
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="X30">
-        <f>COUNTBLANK(E30:W30)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1585,10 +1585,10 @@
         <v>1512705</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D31" s="8">
         <v>6</v>
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="X31">
-        <f>COUNTBLANK(E31:W31)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1607,17 +1607,17 @@
         <v>1513489</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="D32" s="8">
         <v>6</v>
       </c>
       <c r="E32" s="6"/>
       <c r="X32">
-        <f>COUNTBLANK(E32:W32)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1626,10 +1626,10 @@
         <v>1513505</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="D33" s="8">
         <v>6</v>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="X33">
-        <f>COUNTBLANK(E33:W33)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1648,10 +1648,10 @@
         <v>1533720</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="D34" s="8">
         <v>6</v>
@@ -1661,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="X34">
-        <f>COUNTBLANK(E34:W34)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -1670,17 +1670,17 @@
         <v>1410285</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="D35" s="8">
         <v>7</v>
       </c>
       <c r="E35" s="6"/>
       <c r="X35">
-        <f>COUNTBLANK(E35:W35)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1689,17 +1689,17 @@
         <v>1410397</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D36" s="8">
         <v>7</v>
       </c>
       <c r="E36" s="6"/>
       <c r="X36">
-        <f>COUNTBLANK(E36:W36)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1708,17 +1708,17 @@
         <v>1412103</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="D37" s="8">
         <v>7</v>
       </c>
       <c r="E37" s="6"/>
       <c r="X37">
-        <f>COUNTBLANK(E37:W37)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
         <v>1512510</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="8">
         <v>7</v>
       </c>
       <c r="E38" s="6"/>
       <c r="X38">
-        <f>COUNTBLANK(E38:W38)</f>
+        <f t="shared" ref="X38:X69" si="1">COUNTBLANK(E38:W38)</f>
         <v>19</v>
       </c>
     </row>
@@ -1746,17 +1746,17 @@
         <v>1413471</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="D39" s="8">
         <v>7</v>
       </c>
       <c r="E39" s="6"/>
       <c r="X39">
-        <f>COUNTBLANK(E39:W39)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1765,10 +1765,10 @@
         <v>1510322</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D40" s="8">
         <v>8</v>
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="X40">
-        <f>COUNTBLANK(E40:W40)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1787,17 +1787,17 @@
         <v>1512022</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="D41" s="8">
         <v>8</v>
       </c>
       <c r="E41" s="6"/>
       <c r="X41">
-        <f>COUNTBLANK(E41:W41)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1806,17 +1806,17 @@
         <v>1512830</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="D42" s="8">
         <v>8</v>
       </c>
       <c r="E42" s="6"/>
       <c r="X42">
-        <f>COUNTBLANK(E42:W42)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1825,17 +1825,17 @@
         <v>1513555</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="D43" s="8">
         <v>8</v>
       </c>
       <c r="E43" s="6"/>
       <c r="X43">
-        <f>COUNTBLANK(E43:W43)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1844,10 +1844,10 @@
         <v>1513776</v>
       </c>
       <c r="B44" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="D44" s="8">
         <v>8</v>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="X44">
-        <f>COUNTBLANK(E44:W44)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1866,10 +1866,10 @@
         <v>1512489</v>
       </c>
       <c r="B45" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="D45" s="8">
         <v>9</v>
@@ -1879,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="X45">
-        <f>COUNTBLANK(E45:W45)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1888,10 +1888,10 @@
         <v>1512579</v>
       </c>
       <c r="B46" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="D46" s="8">
         <v>9</v>
@@ -1903,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="X46">
-        <f>COUNTBLANK(E46:W46)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
@@ -1912,17 +1912,17 @@
         <v>1512702</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" s="8">
         <v>9</v>
       </c>
       <c r="E47" s="6"/>
       <c r="X47">
-        <f>COUNTBLANK(E47:W47)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1931,10 +1931,10 @@
         <v>1512872</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D48" s="8">
         <v>9</v>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="X48">
-        <f>COUNTBLANK(E48:W48)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -1962,10 +1962,10 @@
         <v>1513172</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="D49" s="8">
         <v>9</v>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="X49">
-        <f>COUNTBLANK(E49:W49)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -2005,10 +2005,10 @@
         <v>1513372</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="D50" s="8">
         <v>9</v>
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="X50">
-        <f>COUNTBLANK(E50:W50)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2026,17 +2026,17 @@
         <v>1510042</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="D51" s="8">
         <v>10</v>
       </c>
       <c r="E51" s="6"/>
       <c r="X51">
-        <f>COUNTBLANK(E51:W51)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2045,17 +2045,17 @@
         <v>1510391</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="D52" s="8">
         <v>10</v>
       </c>
       <c r="E52" s="6"/>
       <c r="X52">
-        <f>COUNTBLANK(E52:W52)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2064,10 +2064,10 @@
         <v>1511734</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="8">
         <v>10</v>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="X53">
-        <f>COUNTBLANK(E53:W53)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2086,17 +2086,17 @@
         <v>1513058</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="D54" s="8">
         <v>10</v>
       </c>
       <c r="E54" s="6"/>
       <c r="X54">
-        <f>COUNTBLANK(E54:W54)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2105,17 +2105,17 @@
         <v>1510484</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D55" s="8">
         <v>11</v>
       </c>
       <c r="E55" s="6"/>
       <c r="X55">
-        <f>COUNTBLANK(E55:W55)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2124,17 +2124,17 @@
         <v>1511025</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D56" s="8">
         <v>11</v>
       </c>
       <c r="E56" s="6"/>
       <c r="X56">
-        <f>COUNTBLANK(E56:W56)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2143,17 +2143,17 @@
         <v>1511979</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D57" s="8">
         <v>11</v>
       </c>
       <c r="E57" s="6"/>
       <c r="X57">
-        <f>COUNTBLANK(E57:W57)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2162,10 +2162,10 @@
         <v>1512217</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D58" s="8">
         <v>11</v>
@@ -2175,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="X58">
-        <f>COUNTBLANK(E58:W58)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2184,17 +2184,17 @@
         <v>1513614</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D59" s="8">
         <v>11</v>
       </c>
       <c r="E59" s="6"/>
       <c r="X59">
-        <f>COUNTBLANK(E59:W59)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2203,10 +2203,10 @@
         <v>1410178</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="D60" s="8">
         <v>12</v>
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="X60">
-        <f>COUNTBLANK(E60:W60)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2225,10 +2225,10 @@
         <v>1510274</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="D61" s="8">
         <v>12</v>
@@ -2238,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="X61">
-        <f>COUNTBLANK(E61:W61)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2247,17 +2247,17 @@
         <v>1511440</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D62" s="8">
         <v>12</v>
       </c>
       <c r="E62" s="6"/>
       <c r="X62">
-        <f>COUNTBLANK(E62:W62)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2266,17 +2266,17 @@
         <v>1411801</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="D63" s="8">
         <v>12</v>
       </c>
       <c r="E63" s="6"/>
       <c r="X63">
-        <f>COUNTBLANK(E63:W63)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2285,10 +2285,10 @@
         <v>1610811</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="D64" s="8">
         <v>13</v>
@@ -2298,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="X64">
-        <f>COUNTBLANK(E64:W64)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2307,17 +2307,17 @@
         <v>1620052</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D65" s="8">
         <v>13</v>
       </c>
       <c r="E65" s="6"/>
       <c r="X65">
-        <f>COUNTBLANK(E65:W65)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2326,17 +2326,17 @@
         <v>1513467</v>
       </c>
       <c r="B66" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="D66" s="8">
         <v>13</v>
       </c>
       <c r="E66" s="6"/>
       <c r="X66">
-        <f>COUNTBLANK(E66:W66)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2345,17 +2345,17 @@
         <v>1510332</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D67" s="8">
         <v>14</v>
       </c>
       <c r="E67" s="6"/>
       <c r="X67">
-        <f>COUNTBLANK(E67:W67)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2364,17 +2364,17 @@
         <v>1510830</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="D68" s="8">
         <v>14</v>
       </c>
       <c r="E68" s="6"/>
       <c r="X68">
-        <f>COUNTBLANK(E68:W68)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2383,17 +2383,17 @@
         <v>1512296</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="D69" s="8">
         <v>14</v>
       </c>
       <c r="E69" s="6"/>
       <c r="X69">
-        <f>COUNTBLANK(E69:W69)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2402,17 +2402,17 @@
         <v>1512312</v>
       </c>
       <c r="B70" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="D70" s="8">
         <v>14</v>
       </c>
       <c r="E70" s="6"/>
       <c r="X70">
-        <f>COUNTBLANK(E70:W70)</f>
+        <f t="shared" ref="X70:X101" si="2">COUNTBLANK(E70:W70)</f>
         <v>19</v>
       </c>
     </row>
@@ -2421,17 +2421,17 @@
         <v>1511013</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D71" s="8">
         <v>15</v>
       </c>
       <c r="E71" s="6"/>
       <c r="X71">
-        <f>COUNTBLANK(E71:W71)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2440,17 +2440,17 @@
         <v>1511552</v>
       </c>
       <c r="B72" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="D72" s="8">
         <v>15</v>
       </c>
       <c r="E72" s="6"/>
       <c r="X72">
-        <f>COUNTBLANK(E72:W72)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
         <v>1513157</v>
       </c>
       <c r="B73" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="D73" s="8">
         <v>15</v>
       </c>
       <c r="E73" s="6"/>
       <c r="X73">
-        <f>COUNTBLANK(E73:W73)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2478,17 +2478,17 @@
         <v>1410947</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D74" s="8">
         <v>15</v>
       </c>
       <c r="E74" s="6"/>
       <c r="X74">
-        <f>COUNTBLANK(E74:W74)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>

</xml_diff>